<commit_message>
Fix UI bugs, improve POS client selection, and fix data type errors in customers/suppliers modules
</commit_message>
<xml_diff>
--- a/data/backup.xlsx
+++ b/data/backup.xlsx
@@ -506,7 +506,7 @@
         <v>50000</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,6 +607,46 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>2025-12-22 23:43:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>VNT-20251223011259-1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-12-23 00:12:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VNT-20251223011405-1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-12-23 00:14:05</t>
         </is>
       </c>
     </row>
@@ -681,10 +721,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>50000</v>
+        <v>49000</v>
       </c>
       <c r="D3" t="n">
-        <v>50000</v>
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>